<commit_message>
fix for importer and more tests
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/import/valid_teams_invalid_athletes.xlsx
+++ b/spec/fixtures/files/import/valid_teams_invalid_athletes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Jersey Number</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -320,7 +323,7 @@
   <dimension ref="A1:V52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="A2:I2 A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -583,10 +586,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="A2:I2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -625,6 +628,11 @@
         <v>44</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>